<commit_message>
Fix port and excel warnings
</commit_message>
<xml_diff>
--- a/static/Mesures.xlsx
+++ b/static/Mesures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GIGABYTE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\flask_app -MVC\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FC2EE5-BB18-43E9-90B3-70C6A998DAF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AB6A75-F906-43E3-8C5E-066157AE2B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="14" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="15" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NABEUL" sheetId="2" r:id="rId1"/>
@@ -3965,33 +3965,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4004,6 +3977,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4012,6 +3991,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4022,7 +4022,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4034,13 +4040,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4337,8 +4337,8 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5673,31 +5673,6 @@
     <mergeCell ref="C23:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{4A629B41-5B0F-421A-93EE-870DF8A1E00A}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7887,31 +7862,6 @@
     <mergeCell ref="C47:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{A85F3CFB-59E4-4E7A-97F6-311821BADC85}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K56</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9759,31 +9709,6 @@
     <mergeCell ref="C22:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{66E65420-4183-4A10-A11D-B5C9FC903846}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K46</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11972,31 +11897,6 @@
     <mergeCell ref="C41:C46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{206D9DB2-6FBD-4275-96DE-BC5146AC7112}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K56</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -14172,44 +14072,19 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C22:C26"/>
     <mergeCell ref="C52:C56"/>
     <mergeCell ref="C27:C31"/>
     <mergeCell ref="C32:C36"/>
     <mergeCell ref="C37:C41"/>
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="C47:C51"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="C22:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{2460A65D-7979-4AE5-B0AB-D5B52F4DF216}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K56</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -16783,31 +16658,6 @@
     <mergeCell ref="C37:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{2BE3BDA9-A91A-4875-A9A8-4F005E958476}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K66</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -19172,11 +19022,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="C22:C26"/>
     <mergeCell ref="C57:C61"/>
     <mergeCell ref="C27:C31"/>
     <mergeCell ref="C32:C36"/>
@@ -19184,33 +19029,13 @@
     <mergeCell ref="C42:C46"/>
     <mergeCell ref="C47:C51"/>
     <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="C22:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{DB0D719D-05D4-4A03-BA2A-15E93E0BED0A}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K61</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -21020,31 +20845,6 @@
     <mergeCell ref="C22:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{0221515A-BAC4-4412-BFCD-1534F994C895}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K46</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -22450,31 +22250,6 @@
     <mergeCell ref="C25:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{1E7A96D0-5706-4D5E-86DB-824FC4C3AA6D}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -24592,44 +24367,19 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="C38:C41"/>
     <mergeCell ref="C28:C32"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="C7:C11"/>
     <mergeCell ref="C12:C16"/>
     <mergeCell ref="C17:C22"/>
     <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="C38:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{AC86BF02-D6BC-4905-A4E9-49E2A0F2BEC7}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K56</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -25710,31 +25460,6 @@
     <mergeCell ref="C19:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{FE0069D0-1C62-4870-897C-E0C78D2C132B}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K26</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -27185,31 +26910,6 @@
     <mergeCell ref="C27:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{84F0AB21-ADBF-45C5-A9D7-F577847B2781}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -28405,31 +28105,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{79A6B801-2414-4E84-8198-ADA9889C839F}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K31</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -28486,7 +28161,7 @@
       <c r="A2" s="69" t="s">
         <v>972</v>
       </c>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="73" t="s">
         <v>973</v>
       </c>
       <c r="C2" s="70">
@@ -28510,10 +28185,10 @@
         <f t="shared" ref="H2:H36" si="1">ROUND(F2*15%,0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I2" s="85">
+      <c r="I2" s="76">
         <v>45082</v>
       </c>
-      <c r="J2" s="86">
+      <c r="J2" s="79">
         <v>2</v>
       </c>
       <c r="K2" s="4">
@@ -28525,7 +28200,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="69"/>
-      <c r="B3" s="83"/>
+      <c r="B3" s="74"/>
       <c r="C3" s="65"/>
       <c r="D3" s="4" t="s">
         <v>974</v>
@@ -28545,8 +28220,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="87"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="4">
         <v>1</v>
       </c>
@@ -28556,7 +28231,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="69"/>
-      <c r="B4" s="83"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="65"/>
       <c r="D4" s="4" t="s">
         <v>975</v>
@@ -28576,8 +28251,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="87"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="4">
         <v>1</v>
       </c>
@@ -28587,7 +28262,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="69"/>
-      <c r="B5" s="83"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="65"/>
       <c r="D5" s="4" t="s">
         <v>976</v>
@@ -28607,8 +28282,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="87"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="4">
         <v>1</v>
       </c>
@@ -28618,7 +28293,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69"/>
-      <c r="B6" s="84"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="71"/>
       <c r="D6" s="7" t="s">
         <v>977</v>
@@ -28638,8 +28313,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="88"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="81"/>
       <c r="K6" s="4">
         <v>1</v>
       </c>
@@ -28649,7 +28324,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="69"/>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="73" t="s">
         <v>978</v>
       </c>
       <c r="C7" s="70">
@@ -28673,10 +28348,10 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="85">
+      <c r="I7" s="76">
         <v>45083</v>
       </c>
-      <c r="J7" s="73">
+      <c r="J7" s="82">
         <v>2</v>
       </c>
       <c r="K7" s="4">
@@ -28688,7 +28363,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="69"/>
-      <c r="B8" s="83"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="65"/>
       <c r="D8" s="4" t="s">
         <v>979</v>
@@ -28708,8 +28383,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
       <c r="K8" s="4">
         <v>1</v>
       </c>
@@ -28719,7 +28394,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="69"/>
-      <c r="B9" s="83"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="65"/>
       <c r="D9" s="4" t="s">
         <v>980</v>
@@ -28739,8 +28414,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
       <c r="K9" s="4">
         <v>1</v>
       </c>
@@ -28750,7 +28425,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="69"/>
-      <c r="B10" s="83"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="65"/>
       <c r="D10" s="4" t="s">
         <v>981</v>
@@ -28770,8 +28445,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
       <c r="K10" s="4">
         <v>1</v>
       </c>
@@ -28781,7 +28456,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
-      <c r="B11" s="84"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="71"/>
       <c r="D11" s="7" t="s">
         <v>982</v>
@@ -28801,8 +28476,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
       <c r="K11" s="4">
         <v>1</v>
       </c>
@@ -28812,7 +28487,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="69"/>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="73" t="s">
         <v>983</v>
       </c>
       <c r="C12" s="70">
@@ -28836,10 +28511,10 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="76">
         <v>45084</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="82">
         <v>2</v>
       </c>
       <c r="K12" s="4">
@@ -28851,7 +28526,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="69"/>
-      <c r="B13" s="83"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="65"/>
       <c r="D13" s="4" t="s">
         <v>984</v>
@@ -28871,8 +28546,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="77"/>
       <c r="K13" s="4">
         <v>1</v>
       </c>
@@ -28882,7 +28557,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="69"/>
-      <c r="B14" s="83"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="65"/>
       <c r="D14" s="4" t="s">
         <v>985</v>
@@ -28902,8 +28577,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
       <c r="K14" s="4">
         <v>1</v>
       </c>
@@ -28913,7 +28588,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="69"/>
-      <c r="B15" s="83"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="65"/>
       <c r="D15" s="4" t="s">
         <v>986</v>
@@ -28933,8 +28608,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
       <c r="K15" s="4">
         <v>1</v>
       </c>
@@ -28944,7 +28619,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="69"/>
-      <c r="B16" s="84"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="71"/>
       <c r="D16" s="7" t="s">
         <v>987</v>
@@ -28964,8 +28639,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
       <c r="K16" s="4">
         <v>1</v>
       </c>
@@ -28975,7 +28650,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="69"/>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="73" t="s">
         <v>988</v>
       </c>
       <c r="C17" s="70">
@@ -28999,10 +28674,10 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I17" s="79">
+      <c r="I17" s="83">
         <v>45085</v>
       </c>
-      <c r="J17" s="73">
+      <c r="J17" s="82">
         <v>2</v>
       </c>
       <c r="K17" s="4">
@@ -29014,7 +28689,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="69"/>
-      <c r="B18" s="83"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="65"/>
       <c r="D18" s="4" t="s">
         <v>990</v>
@@ -29034,8 +28709,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I18" s="80"/>
-      <c r="J18" s="74"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="77"/>
       <c r="K18" s="4">
         <v>1</v>
       </c>
@@ -29045,7 +28720,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="69"/>
-      <c r="B19" s="83"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="65"/>
       <c r="D19" s="4" t="s">
         <v>991</v>
@@ -29065,8 +28740,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I19" s="80"/>
-      <c r="J19" s="74"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="77"/>
       <c r="K19" s="4">
         <v>1</v>
       </c>
@@ -29076,7 +28751,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="69"/>
-      <c r="B20" s="83"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="65"/>
       <c r="D20" s="4" t="s">
         <v>992</v>
@@ -29096,8 +28771,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I20" s="80"/>
-      <c r="J20" s="74"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="77"/>
       <c r="K20" s="4">
         <v>1</v>
       </c>
@@ -29107,7 +28782,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="69"/>
-      <c r="B21" s="84"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="71"/>
       <c r="D21" s="7" t="s">
         <v>993</v>
@@ -29127,8 +28802,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" s="81"/>
-      <c r="J21" s="75"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="78"/>
       <c r="K21" s="4">
         <v>1</v>
       </c>
@@ -29138,7 +28813,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="69"/>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="73" t="s">
         <v>994</v>
       </c>
       <c r="C22" s="70">
@@ -29162,10 +28837,10 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I22" s="79">
+      <c r="I22" s="83">
         <v>45086</v>
       </c>
-      <c r="J22" s="73">
+      <c r="J22" s="82">
         <v>2</v>
       </c>
       <c r="K22" s="4">
@@ -29177,7 +28852,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="69"/>
-      <c r="B23" s="83"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="65"/>
       <c r="D23" s="4" t="s">
         <v>995</v>
@@ -29197,8 +28872,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I23" s="80"/>
-      <c r="J23" s="74"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="77"/>
       <c r="K23" s="4">
         <v>1</v>
       </c>
@@ -29208,7 +28883,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="69"/>
-      <c r="B24" s="83"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="65"/>
       <c r="D24" s="4" t="s">
         <v>996</v>
@@ -29228,8 +28903,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I24" s="80"/>
-      <c r="J24" s="74"/>
+      <c r="I24" s="84"/>
+      <c r="J24" s="77"/>
       <c r="K24" s="4">
         <v>1</v>
       </c>
@@ -29239,7 +28914,7 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="69"/>
-      <c r="B25" s="83"/>
+      <c r="B25" s="74"/>
       <c r="C25" s="65"/>
       <c r="D25" s="4" t="s">
         <v>997</v>
@@ -29259,8 +28934,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I25" s="80"/>
-      <c r="J25" s="74"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="77"/>
       <c r="K25" s="4">
         <v>1</v>
       </c>
@@ -29270,7 +28945,7 @@
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="69"/>
-      <c r="B26" s="84"/>
+      <c r="B26" s="75"/>
       <c r="C26" s="71"/>
       <c r="D26" s="7" t="s">
         <v>998</v>
@@ -29290,8 +28965,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I26" s="81"/>
-      <c r="J26" s="75"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="78"/>
       <c r="K26" s="4">
         <v>1</v>
       </c>
@@ -29301,7 +28976,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="69"/>
-      <c r="B27" s="82" t="s">
+      <c r="B27" s="73" t="s">
         <v>999</v>
       </c>
       <c r="C27" s="70">
@@ -29325,10 +29000,10 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I27" s="79">
+      <c r="I27" s="83">
         <v>45089</v>
       </c>
-      <c r="J27" s="73">
+      <c r="J27" s="82">
         <v>2</v>
       </c>
       <c r="K27" s="4">
@@ -29340,7 +29015,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="69"/>
-      <c r="B28" s="83"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="65"/>
       <c r="D28" s="4" t="s">
         <v>1000</v>
@@ -29360,8 +29035,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" s="80"/>
-      <c r="J28" s="74"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="77"/>
       <c r="K28" s="4">
         <v>1</v>
       </c>
@@ -29371,7 +29046,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="69"/>
-      <c r="B29" s="83"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="65"/>
       <c r="D29" s="4" t="s">
         <v>1001</v>
@@ -29391,8 +29066,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I29" s="80"/>
-      <c r="J29" s="74"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="77"/>
       <c r="K29" s="4">
         <v>1</v>
       </c>
@@ -29402,7 +29077,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="69"/>
-      <c r="B30" s="83"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="65"/>
       <c r="D30" s="4" t="s">
         <v>1002</v>
@@ -29422,8 +29097,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I30" s="80"/>
-      <c r="J30" s="74"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="77"/>
       <c r="K30" s="4">
         <v>1</v>
       </c>
@@ -29433,7 +29108,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="69"/>
-      <c r="B31" s="84"/>
+      <c r="B31" s="75"/>
       <c r="C31" s="71"/>
       <c r="D31" s="7" t="s">
         <v>1003</v>
@@ -29453,8 +29128,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I31" s="81"/>
-      <c r="J31" s="75"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="78"/>
       <c r="K31" s="4">
         <v>1</v>
       </c>
@@ -29464,7 +29139,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="69"/>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="86" t="s">
         <v>1004</v>
       </c>
       <c r="C32" s="70">
@@ -29488,10 +29163,10 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I32" s="79">
+      <c r="I32" s="83">
         <v>45090</v>
       </c>
-      <c r="J32" s="73">
+      <c r="J32" s="82">
         <v>2</v>
       </c>
       <c r="K32" s="4">
@@ -29503,7 +29178,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="69"/>
-      <c r="B33" s="77"/>
+      <c r="B33" s="87"/>
       <c r="C33" s="65"/>
       <c r="D33" s="4" t="s">
         <v>1005</v>
@@ -29523,8 +29198,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I33" s="80"/>
-      <c r="J33" s="74"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="77"/>
       <c r="K33" s="4">
         <v>1</v>
       </c>
@@ -29534,7 +29209,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="69"/>
-      <c r="B34" s="77"/>
+      <c r="B34" s="87"/>
       <c r="C34" s="65"/>
       <c r="D34" s="4" t="s">
         <v>1006</v>
@@ -29554,8 +29229,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I34" s="80"/>
-      <c r="J34" s="74"/>
+      <c r="I34" s="84"/>
+      <c r="J34" s="77"/>
       <c r="K34" s="4">
         <v>1</v>
       </c>
@@ -29565,7 +29240,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="69"/>
-      <c r="B35" s="77"/>
+      <c r="B35" s="87"/>
       <c r="C35" s="65"/>
       <c r="D35" s="4" t="s">
         <v>1007</v>
@@ -29585,8 +29260,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I35" s="80"/>
-      <c r="J35" s="74"/>
+      <c r="I35" s="84"/>
+      <c r="J35" s="77"/>
       <c r="K35" s="4">
         <v>1</v>
       </c>
@@ -29596,7 +29271,7 @@
     </row>
     <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="69"/>
-      <c r="B36" s="78"/>
+      <c r="B36" s="88"/>
       <c r="C36" s="71"/>
       <c r="D36" s="7" t="s">
         <v>1008</v>
@@ -29616,8 +29291,8 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I36" s="81"/>
-      <c r="J36" s="74"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="77"/>
       <c r="K36" s="4">
         <v>1</v>
       </c>
@@ -29627,6 +29302,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="J27:J31"/>
     <mergeCell ref="A2:A36"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
@@ -29643,370 +29331,9 @@
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="I17:I21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="J32:J36"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="J27:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="18" id="{53D4C904-8CD8-4CA1-86C3-EE1F42A295FA}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="17" id="{4AC7B5EB-5367-45C9-9B92-DE5CD0F4E8D4}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K3:K6</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="16" id="{82FD9EBE-AD43-4301-A2C6-AB0D84C32DA5}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K7</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="13" id="{9CDA351E-C978-4344-9912-9C058065AA55}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{0DC5FFE8-1BB5-4295-9EBE-843CE946E2D3}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{E818EE03-D713-4FBD-AB66-3FBE8AD45434}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K10</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="14" id="{1558AD58-052F-446D-9016-26DFA2EBD415}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="11" id="{25E1715B-2006-4343-A34D-01593A5FE167}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K12</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{9D57C1D7-B658-4706-B4AD-8300B2556009}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K13</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{AFB14E52-A3C3-422E-B93E-809EEE85B92A}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K14</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="9" id="{853CFF84-0BFE-4983-9EFB-E8C20B1198AF}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K15</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="10" id="{0FF3E4DD-1359-4453-900A-F29D8D9BFD74}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{F90CFB01-827E-4DA7-818D-C95D23C350AF}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K17</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{4AB48EE1-0471-4A49-98AD-88E23A043D0E}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{5D7DBC2F-9175-476F-A97C-23B101C96CB2}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{7819422E-39F6-4373-97F8-B315A4FBFFEF}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K20</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{12D18CB8-C48F-4285-980B-5DAD34CC81B8}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K21</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{3A87A4D4-CD0C-4C78-A2F2-01060689C630}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K22:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -30060,7 +29387,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="95" t="s">
         <v>1009</v>
       </c>
       <c r="B2" s="89" t="s">
@@ -30086,7 +29413,7 @@
         <f t="shared" ref="H2:H36" si="1">ROUND(F2*15%,0)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="96">
+      <c r="I2" s="92">
         <v>45092</v>
       </c>
       <c r="J2" s="69">
@@ -30100,7 +29427,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="94"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="90"/>
       <c r="C3" s="65"/>
       <c r="D3" s="4" t="s">
@@ -30120,7 +29447,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I3" s="97"/>
+      <c r="I3" s="93"/>
       <c r="J3" s="69"/>
       <c r="K3" s="4">
         <v>1</v>
@@ -30130,7 +29457,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="94"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="90"/>
       <c r="C4" s="65"/>
       <c r="D4" s="4" t="s">
@@ -30150,7 +29477,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I4" s="97"/>
+      <c r="I4" s="93"/>
       <c r="J4" s="69"/>
       <c r="K4" s="4">
         <v>1</v>
@@ -30160,7 +29487,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="94"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="90"/>
       <c r="C5" s="65"/>
       <c r="D5" s="4" t="s">
@@ -30180,7 +29507,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I5" s="97"/>
+      <c r="I5" s="93"/>
       <c r="J5" s="69"/>
       <c r="K5" s="4">
         <v>1</v>
@@ -30190,7 +29517,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="94"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="91"/>
       <c r="C6" s="66"/>
       <c r="D6" s="4" t="s">
@@ -30210,7 +29537,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I6" s="98"/>
+      <c r="I6" s="94"/>
       <c r="J6" s="69"/>
       <c r="K6" s="4">
         <v>1</v>
@@ -30220,7 +29547,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="94"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="89" t="s">
         <v>1015</v>
       </c>
@@ -30244,7 +29571,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I7" s="96">
+      <c r="I7" s="92">
         <v>45093</v>
       </c>
       <c r="J7" s="69">
@@ -30258,7 +29585,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="94"/>
+      <c r="A8" s="96"/>
       <c r="B8" s="90"/>
       <c r="C8" s="65"/>
       <c r="D8" s="4" t="s">
@@ -30278,7 +29605,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I8" s="97"/>
+      <c r="I8" s="93"/>
       <c r="J8" s="69"/>
       <c r="K8" s="4">
         <v>1</v>
@@ -30288,7 +29615,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="94"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="90"/>
       <c r="C9" s="65"/>
       <c r="D9" s="4" t="s">
@@ -30308,7 +29635,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I9" s="97"/>
+      <c r="I9" s="93"/>
       <c r="J9" s="69"/>
       <c r="K9" s="4">
         <v>1</v>
@@ -30318,7 +29645,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="94"/>
+      <c r="A10" s="96"/>
       <c r="B10" s="90"/>
       <c r="C10" s="65"/>
       <c r="D10" s="4" t="s">
@@ -30338,7 +29665,7 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I10" s="97"/>
+      <c r="I10" s="93"/>
       <c r="J10" s="69"/>
       <c r="K10" s="4">
         <v>1</v>
@@ -30348,7 +29675,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="94"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="91"/>
       <c r="C11" s="66"/>
       <c r="D11" s="4" t="s">
@@ -30368,7 +29695,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I11" s="98"/>
+      <c r="I11" s="94"/>
       <c r="J11" s="69"/>
       <c r="K11" s="4">
         <v>1</v>
@@ -30378,7 +29705,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="94"/>
+      <c r="A12" s="96"/>
       <c r="B12" s="89" t="s">
         <v>1021</v>
       </c>
@@ -30402,7 +29729,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I12" s="96">
+      <c r="I12" s="92">
         <v>45096</v>
       </c>
       <c r="J12" s="69">
@@ -30416,7 +29743,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="94"/>
+      <c r="A13" s="96"/>
       <c r="B13" s="90"/>
       <c r="C13" s="65"/>
       <c r="D13" s="4" t="s">
@@ -30436,7 +29763,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I13" s="97"/>
+      <c r="I13" s="93"/>
       <c r="J13" s="69"/>
       <c r="K13" s="4">
         <v>1</v>
@@ -30446,7 +29773,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="94"/>
+      <c r="A14" s="96"/>
       <c r="B14" s="90"/>
       <c r="C14" s="65"/>
       <c r="D14" s="4" t="s">
@@ -30466,7 +29793,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I14" s="97"/>
+      <c r="I14" s="93"/>
       <c r="J14" s="69"/>
       <c r="K14" s="4">
         <v>1</v>
@@ -30476,7 +29803,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="94"/>
+      <c r="A15" s="96"/>
       <c r="B15" s="90"/>
       <c r="C15" s="65"/>
       <c r="D15" s="4" t="s">
@@ -30496,7 +29823,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I15" s="97"/>
+      <c r="I15" s="93"/>
       <c r="J15" s="69"/>
       <c r="K15" s="4">
         <v>1</v>
@@ -30506,7 +29833,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="94"/>
+      <c r="A16" s="96"/>
       <c r="B16" s="91"/>
       <c r="C16" s="66"/>
       <c r="D16" s="4" t="s">
@@ -30526,7 +29853,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I16" s="98"/>
+      <c r="I16" s="94"/>
       <c r="J16" s="69"/>
       <c r="K16" s="4">
         <v>1</v>
@@ -30536,7 +29863,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="94"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="89" t="s">
         <v>1027</v>
       </c>
@@ -30560,7 +29887,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I17" s="96">
+      <c r="I17" s="92">
         <v>45097</v>
       </c>
       <c r="J17" s="69">
@@ -30574,7 +29901,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="94"/>
+      <c r="A18" s="96"/>
       <c r="B18" s="90"/>
       <c r="C18" s="65"/>
       <c r="D18" s="4" t="s">
@@ -30594,7 +29921,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I18" s="92"/>
+      <c r="I18" s="98"/>
       <c r="J18" s="69"/>
       <c r="K18" s="4">
         <v>1</v>
@@ -30604,7 +29931,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="94"/>
+      <c r="A19" s="96"/>
       <c r="B19" s="90"/>
       <c r="C19" s="65"/>
       <c r="D19" s="4" t="s">
@@ -30624,7 +29951,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I19" s="92"/>
+      <c r="I19" s="98"/>
       <c r="J19" s="69"/>
       <c r="K19" s="4">
         <v>1</v>
@@ -30634,7 +29961,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="94"/>
+      <c r="A20" s="96"/>
       <c r="B20" s="91"/>
       <c r="C20" s="66"/>
       <c r="D20" s="4" t="s">
@@ -30654,7 +29981,7 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I20" s="92"/>
+      <c r="I20" s="98"/>
       <c r="J20" s="69"/>
       <c r="K20" s="4">
         <v>1</v>
@@ -30664,7 +29991,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="94"/>
+      <c r="A21" s="96"/>
       <c r="B21" s="89" t="s">
         <v>1031</v>
       </c>
@@ -30688,7 +30015,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I21" s="92">
+      <c r="I21" s="98">
         <v>45098</v>
       </c>
       <c r="J21" s="69">
@@ -30702,7 +30029,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="94"/>
+      <c r="A22" s="96"/>
       <c r="B22" s="90"/>
       <c r="C22" s="65"/>
       <c r="D22" s="4" t="s">
@@ -30722,7 +30049,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I22" s="92"/>
+      <c r="I22" s="98"/>
       <c r="J22" s="69"/>
       <c r="K22" s="4">
         <v>1</v>
@@ -30732,7 +30059,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="94"/>
+      <c r="A23" s="96"/>
       <c r="B23" s="90"/>
       <c r="C23" s="65"/>
       <c r="D23" s="4" t="s">
@@ -30752,7 +30079,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I23" s="92"/>
+      <c r="I23" s="98"/>
       <c r="J23" s="69"/>
       <c r="K23" s="4">
         <v>1</v>
@@ -30762,7 +30089,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="94"/>
+      <c r="A24" s="96"/>
       <c r="B24" s="90"/>
       <c r="C24" s="65"/>
       <c r="D24" s="4" t="s">
@@ -30782,7 +30109,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I24" s="92"/>
+      <c r="I24" s="98"/>
       <c r="J24" s="69"/>
       <c r="K24" s="4">
         <v>1</v>
@@ -30792,7 +30119,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="94"/>
+      <c r="A25" s="96"/>
       <c r="B25" s="91"/>
       <c r="C25" s="66"/>
       <c r="D25" s="4" t="s">
@@ -30812,7 +30139,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I25" s="92"/>
+      <c r="I25" s="98"/>
       <c r="J25" s="69"/>
       <c r="K25" s="4">
         <v>1</v>
@@ -30822,7 +30149,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="94"/>
+      <c r="A26" s="96"/>
       <c r="B26" s="89" t="s">
         <v>1037</v>
       </c>
@@ -30846,7 +30173,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I26" s="92">
+      <c r="I26" s="98">
         <v>45099</v>
       </c>
       <c r="J26" s="69">
@@ -30860,7 +30187,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="94"/>
+      <c r="A27" s="96"/>
       <c r="B27" s="90"/>
       <c r="C27" s="65"/>
       <c r="D27" s="4" t="s">
@@ -30880,7 +30207,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I27" s="92"/>
+      <c r="I27" s="98"/>
       <c r="J27" s="69"/>
       <c r="K27" s="4">
         <v>1</v>
@@ -30890,7 +30217,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="94"/>
+      <c r="A28" s="96"/>
       <c r="B28" s="90"/>
       <c r="C28" s="65"/>
       <c r="D28" s="4" t="s">
@@ -30910,7 +30237,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I28" s="92"/>
+      <c r="I28" s="98"/>
       <c r="J28" s="69"/>
       <c r="K28" s="4">
         <v>1</v>
@@ -30920,7 +30247,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="94"/>
+      <c r="A29" s="96"/>
       <c r="B29" s="90"/>
       <c r="C29" s="65"/>
       <c r="D29" s="4" t="s">
@@ -30940,7 +30267,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I29" s="92"/>
+      <c r="I29" s="98"/>
       <c r="J29" s="69"/>
       <c r="K29" s="4">
         <v>1</v>
@@ -30950,7 +30277,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="94"/>
+      <c r="A30" s="96"/>
       <c r="B30" s="91"/>
       <c r="C30" s="66"/>
       <c r="D30" s="4" t="s">
@@ -30970,7 +30297,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I30" s="92"/>
+      <c r="I30" s="98"/>
       <c r="J30" s="69"/>
       <c r="K30" s="4">
         <v>1</v>
@@ -30980,7 +30307,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="94"/>
+      <c r="A31" s="96"/>
       <c r="B31" s="89" t="s">
         <v>1042</v>
       </c>
@@ -31004,7 +30331,7 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I31" s="92">
+      <c r="I31" s="98">
         <v>45002</v>
       </c>
       <c r="J31" s="69">
@@ -31018,7 +30345,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="94"/>
+      <c r="A32" s="96"/>
       <c r="B32" s="90"/>
       <c r="C32" s="65"/>
       <c r="D32" s="4" t="s">
@@ -31038,7 +30365,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I32" s="92"/>
+      <c r="I32" s="98"/>
       <c r="J32" s="69"/>
       <c r="K32" s="4">
         <v>1</v>
@@ -31048,7 +30375,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="94"/>
+      <c r="A33" s="96"/>
       <c r="B33" s="90"/>
       <c r="C33" s="65"/>
       <c r="D33" s="4" t="s">
@@ -31068,7 +30395,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I33" s="92"/>
+      <c r="I33" s="98"/>
       <c r="J33" s="69"/>
       <c r="K33" s="4">
         <v>1</v>
@@ -31078,7 +30405,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="94"/>
+      <c r="A34" s="96"/>
       <c r="B34" s="90"/>
       <c r="C34" s="65"/>
       <c r="D34" s="4" t="s">
@@ -31098,7 +30425,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I34" s="92"/>
+      <c r="I34" s="98"/>
       <c r="J34" s="69"/>
       <c r="K34" s="4">
         <v>1</v>
@@ -31108,7 +30435,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="94"/>
+      <c r="A35" s="96"/>
       <c r="B35" s="90"/>
       <c r="C35" s="65"/>
       <c r="D35" s="4" t="s">
@@ -31128,7 +30455,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I35" s="92"/>
+      <c r="I35" s="98"/>
       <c r="J35" s="69"/>
       <c r="K35" s="4">
         <v>1</v>
@@ -31138,7 +30465,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="95"/>
+      <c r="A36" s="97"/>
       <c r="B36" s="91"/>
       <c r="C36" s="66"/>
       <c r="D36" s="4" t="s">
@@ -31158,8 +30485,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I36" s="92"/>
-      <c r="J36" s="93"/>
+      <c r="I36" s="98"/>
+      <c r="J36" s="95"/>
       <c r="K36" s="4">
         <v>1</v>
       </c>
@@ -31169,14 +30496,11 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="J26:J30"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="I31:I36"/>
+    <mergeCell ref="J31:J36"/>
     <mergeCell ref="A2:A36"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="C17:C20"/>
@@ -31193,38 +30517,16 @@
     <mergeCell ref="I12:I16"/>
     <mergeCell ref="J12:J16"/>
     <mergeCell ref="B2:B6"/>
-    <mergeCell ref="J26:J30"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="I31:I36"/>
-    <mergeCell ref="J31:J36"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="J7:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{A55AE55A-09FC-4B8A-A8A4-3B984300D96E}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -31281,7 +30583,7 @@
       <c r="A2" s="69" t="s">
         <v>1048</v>
       </c>
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="86" t="s">
         <v>1049</v>
       </c>
       <c r="C2" s="70">
@@ -31305,10 +30607,10 @@
         <f>ROUND(F2*15%,0)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="85">
+      <c r="I2" s="76">
         <v>45082</v>
       </c>
-      <c r="J2" s="86">
+      <c r="J2" s="79">
         <v>1</v>
       </c>
       <c r="K2" s="4">
@@ -31320,7 +30622,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="69"/>
-      <c r="B3" s="77"/>
+      <c r="B3" s="87"/>
       <c r="C3" s="65"/>
       <c r="D3" s="4" t="s">
         <v>1050</v>
@@ -31340,8 +30642,8 @@
         <f t="shared" ref="H3:H41" si="1">ROUND(F3*15%,0)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="87"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="80"/>
       <c r="K3" s="4">
         <v>1</v>
       </c>
@@ -31351,7 +30653,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="69"/>
-      <c r="B4" s="77"/>
+      <c r="B4" s="87"/>
       <c r="C4" s="65"/>
       <c r="D4" s="4" t="s">
         <v>996</v>
@@ -31371,8 +30673,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I4" s="74"/>
-      <c r="J4" s="87"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="4">
         <v>1</v>
       </c>
@@ -31382,7 +30684,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="69"/>
-      <c r="B5" s="77"/>
+      <c r="B5" s="87"/>
       <c r="C5" s="65"/>
       <c r="D5" s="4" t="s">
         <v>96</v>
@@ -31402,8 +30704,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="87"/>
+      <c r="I5" s="77"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="4">
         <v>1</v>
       </c>
@@ -31413,7 +30715,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69"/>
-      <c r="B6" s="78"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="71"/>
       <c r="D6" s="7" t="s">
         <v>1051</v>
@@ -31433,8 +30735,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="88"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="81"/>
       <c r="K6" s="4">
         <v>1</v>
       </c>
@@ -31444,7 +30746,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="69"/>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="86" t="s">
         <v>1052</v>
       </c>
       <c r="C7" s="99">
@@ -31468,10 +30770,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I7" s="85">
+      <c r="I7" s="76">
         <v>45083</v>
       </c>
-      <c r="J7" s="86">
+      <c r="J7" s="79">
         <v>1</v>
       </c>
       <c r="K7" s="4">
@@ -31483,8 +30785,8 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="69"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="94"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="96"/>
       <c r="D8" s="4" t="s">
         <v>1053</v>
       </c>
@@ -31503,8 +30805,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="74"/>
-      <c r="J8" s="87"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="80"/>
       <c r="K8" s="4">
         <v>1</v>
       </c>
@@ -31514,8 +30816,8 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="69"/>
-      <c r="B9" s="77"/>
-      <c r="C9" s="94"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="96"/>
       <c r="D9" s="4" t="s">
         <v>1054</v>
       </c>
@@ -31534,8 +30836,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I9" s="74"/>
-      <c r="J9" s="87"/>
+      <c r="I9" s="77"/>
+      <c r="J9" s="80"/>
       <c r="K9" s="4">
         <v>1</v>
       </c>
@@ -31545,8 +30847,8 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="69"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="94"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="96"/>
       <c r="D10" s="4" t="s">
         <v>1055</v>
       </c>
@@ -31565,8 +30867,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="87"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="80"/>
       <c r="K10" s="4">
         <v>1</v>
       </c>
@@ -31576,7 +30878,7 @@
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
-      <c r="B11" s="78"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="100"/>
       <c r="D11" s="7" t="s">
         <v>1056</v>
@@ -31596,8 +30898,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I11" s="75"/>
-      <c r="J11" s="88"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="81"/>
       <c r="K11" s="4">
         <v>1</v>
       </c>
@@ -31607,7 +30909,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="69"/>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="86" t="s">
         <v>1057</v>
       </c>
       <c r="C12" s="70">
@@ -31631,10 +30933,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="76">
         <v>45084</v>
       </c>
-      <c r="J12" s="86">
+      <c r="J12" s="79">
         <v>1</v>
       </c>
       <c r="K12" s="4">
@@ -31646,7 +30948,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="69"/>
-      <c r="B13" s="77"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="65"/>
       <c r="D13" s="4" t="s">
         <v>1057</v>
@@ -31666,8 +30968,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="87"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="80"/>
       <c r="K13" s="4">
         <v>1</v>
       </c>
@@ -31677,7 +30979,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="69"/>
-      <c r="B14" s="77"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="65"/>
       <c r="D14" s="4" t="s">
         <v>1059</v>
@@ -31697,8 +30999,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I14" s="74"/>
-      <c r="J14" s="87"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="80"/>
       <c r="K14" s="4">
         <v>1</v>
       </c>
@@ -31708,7 +31010,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="69"/>
-      <c r="B15" s="77"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="65"/>
       <c r="D15" s="4" t="s">
         <v>339</v>
@@ -31728,8 +31030,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="87"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="80"/>
       <c r="K15" s="4">
         <v>1</v>
       </c>
@@ -31739,7 +31041,7 @@
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="69"/>
-      <c r="B16" s="78"/>
+      <c r="B16" s="88"/>
       <c r="C16" s="71"/>
       <c r="D16" s="7" t="s">
         <v>1060</v>
@@ -31759,8 +31061,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I16" s="75"/>
-      <c r="J16" s="88"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="81"/>
       <c r="K16" s="4">
         <v>1</v>
       </c>
@@ -31770,7 +31072,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="69"/>
-      <c r="B17" s="76" t="s">
+      <c r="B17" s="86" t="s">
         <v>1061</v>
       </c>
       <c r="C17" s="70">
@@ -31794,10 +31096,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I17" s="85">
+      <c r="I17" s="76">
         <v>45085</v>
       </c>
-      <c r="J17" s="86">
+      <c r="J17" s="79">
         <v>1</v>
       </c>
       <c r="K17" s="4">
@@ -31809,7 +31111,7 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="69"/>
-      <c r="B18" s="77"/>
+      <c r="B18" s="87"/>
       <c r="C18" s="65"/>
       <c r="D18" s="4" t="s">
         <v>1062</v>
@@ -31829,8 +31131,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I18" s="74"/>
-      <c r="J18" s="87"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="80"/>
       <c r="K18" s="4">
         <v>1</v>
       </c>
@@ -31840,7 +31142,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="69"/>
-      <c r="B19" s="77"/>
+      <c r="B19" s="87"/>
       <c r="C19" s="65"/>
       <c r="D19" s="4" t="s">
         <v>1063</v>
@@ -31860,8 +31162,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I19" s="74"/>
-      <c r="J19" s="87"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="80"/>
       <c r="K19" s="4">
         <v>1</v>
       </c>
@@ -31871,7 +31173,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="69"/>
-      <c r="B20" s="77"/>
+      <c r="B20" s="87"/>
       <c r="C20" s="65"/>
       <c r="D20" s="4" t="s">
         <v>1064</v>
@@ -31891,8 +31193,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I20" s="74"/>
-      <c r="J20" s="87"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="80"/>
       <c r="K20" s="4">
         <v>1</v>
       </c>
@@ -31902,7 +31204,7 @@
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="69"/>
-      <c r="B21" s="78"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="71"/>
       <c r="D21" s="7" t="s">
         <v>1065</v>
@@ -31922,8 +31224,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I21" s="75"/>
-      <c r="J21" s="88"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="81"/>
       <c r="K21" s="4">
         <v>1</v>
       </c>
@@ -31933,7 +31235,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="69"/>
-      <c r="B22" s="76" t="s">
+      <c r="B22" s="86" t="s">
         <v>1066</v>
       </c>
       <c r="C22" s="99">
@@ -31957,10 +31259,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I22" s="85">
+      <c r="I22" s="76">
         <v>45086</v>
       </c>
-      <c r="J22" s="86">
+      <c r="J22" s="79">
         <v>1</v>
       </c>
       <c r="K22" s="4">
@@ -31972,8 +31274,8 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="69"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="96"/>
       <c r="D23" s="4" t="s">
         <v>1068</v>
       </c>
@@ -31992,8 +31294,8 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I23" s="74"/>
-      <c r="J23" s="87"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="80"/>
       <c r="K23" s="4">
         <v>1</v>
       </c>
@@ -32003,8 +31305,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="69"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="94"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="96"/>
       <c r="D24" s="4" t="s">
         <v>1069</v>
       </c>
@@ -32023,8 +31325,8 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I24" s="74"/>
-      <c r="J24" s="87"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="80"/>
       <c r="K24" s="4">
         <v>1</v>
       </c>
@@ -32034,8 +31336,8 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="69"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="94"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="96"/>
       <c r="D25" s="4" t="s">
         <v>1070</v>
       </c>
@@ -32054,8 +31356,8 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I25" s="74"/>
-      <c r="J25" s="87"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="80"/>
       <c r="K25" s="4">
         <v>1</v>
       </c>
@@ -32065,7 +31367,7 @@
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="69"/>
-      <c r="B26" s="78"/>
+      <c r="B26" s="88"/>
       <c r="C26" s="100"/>
       <c r="D26" s="7" t="s">
         <v>1071</v>
@@ -32085,8 +31387,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I26" s="75"/>
-      <c r="J26" s="88"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="81"/>
       <c r="K26" s="4">
         <v>1</v>
       </c>
@@ -32096,7 +31398,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="69"/>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="86" t="s">
         <v>1072</v>
       </c>
       <c r="C27" s="70">
@@ -32120,10 +31422,10 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I27" s="85">
+      <c r="I27" s="76">
         <v>45089</v>
       </c>
-      <c r="J27" s="86">
+      <c r="J27" s="79">
         <v>1</v>
       </c>
       <c r="K27" s="4">
@@ -32135,7 +31437,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="69"/>
-      <c r="B28" s="77"/>
+      <c r="B28" s="87"/>
       <c r="C28" s="65"/>
       <c r="D28" s="4" t="s">
         <v>1074</v>
@@ -32155,8 +31457,8 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I28" s="74"/>
-      <c r="J28" s="87"/>
+      <c r="I28" s="77"/>
+      <c r="J28" s="80"/>
       <c r="K28" s="4">
         <v>1</v>
       </c>
@@ -32166,7 +31468,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="69"/>
-      <c r="B29" s="77"/>
+      <c r="B29" s="87"/>
       <c r="C29" s="65"/>
       <c r="D29" s="4" t="s">
         <v>555</v>
@@ -32186,8 +31488,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I29" s="74"/>
-      <c r="J29" s="87"/>
+      <c r="I29" s="77"/>
+      <c r="J29" s="80"/>
       <c r="K29" s="4">
         <v>1</v>
       </c>
@@ -32197,7 +31499,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="69"/>
-      <c r="B30" s="77"/>
+      <c r="B30" s="87"/>
       <c r="C30" s="65"/>
       <c r="D30" s="4" t="s">
         <v>1075</v>
@@ -32217,8 +31519,8 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I30" s="74"/>
-      <c r="J30" s="87"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="80"/>
       <c r="K30" s="4">
         <v>1</v>
       </c>
@@ -32228,7 +31530,7 @@
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="69"/>
-      <c r="B31" s="78"/>
+      <c r="B31" s="88"/>
       <c r="C31" s="71"/>
       <c r="D31" s="7" t="s">
         <v>1076</v>
@@ -32248,8 +31550,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I31" s="75"/>
-      <c r="J31" s="88"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="81"/>
       <c r="K31" s="4">
         <v>1</v>
       </c>
@@ -32259,7 +31561,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="69"/>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="86" t="s">
         <v>1077</v>
       </c>
       <c r="C32" s="70">
@@ -32283,10 +31585,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I32" s="85">
+      <c r="I32" s="76">
         <v>45090</v>
       </c>
-      <c r="J32" s="86">
+      <c r="J32" s="79">
         <v>1</v>
       </c>
       <c r="K32" s="4">
@@ -32298,7 +31600,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="69"/>
-      <c r="B33" s="77"/>
+      <c r="B33" s="87"/>
       <c r="C33" s="65"/>
       <c r="D33" s="4" t="s">
         <v>1078</v>
@@ -32318,8 +31620,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I33" s="74"/>
-      <c r="J33" s="87"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="80"/>
       <c r="K33" s="4">
         <v>1</v>
       </c>
@@ -32329,7 +31631,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="69"/>
-      <c r="B34" s="77"/>
+      <c r="B34" s="87"/>
       <c r="C34" s="65"/>
       <c r="D34" s="4" t="s">
         <v>1079</v>
@@ -32349,8 +31651,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I34" s="74"/>
-      <c r="J34" s="87"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="80"/>
       <c r="K34" s="4">
         <v>1</v>
       </c>
@@ -32360,7 +31662,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="69"/>
-      <c r="B35" s="77"/>
+      <c r="B35" s="87"/>
       <c r="C35" s="65"/>
       <c r="D35" s="4" t="s">
         <v>1080</v>
@@ -32380,8 +31682,8 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I35" s="74"/>
-      <c r="J35" s="87"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="80"/>
       <c r="K35" s="4">
         <v>1</v>
       </c>
@@ -32391,7 +31693,7 @@
     </row>
     <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="69"/>
-      <c r="B36" s="78"/>
+      <c r="B36" s="88"/>
       <c r="C36" s="71"/>
       <c r="D36" s="7" t="s">
         <v>1081</v>
@@ -32411,8 +31713,8 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I36" s="75"/>
-      <c r="J36" s="88"/>
+      <c r="I36" s="78"/>
+      <c r="J36" s="81"/>
       <c r="K36" s="4">
         <v>1</v>
       </c>
@@ -32422,7 +31724,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="69"/>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="86" t="s">
         <v>1082</v>
       </c>
       <c r="C37" s="70">
@@ -32446,10 +31748,10 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I37" s="85">
+      <c r="I37" s="76">
         <v>45091</v>
       </c>
-      <c r="J37" s="86">
+      <c r="J37" s="79">
         <v>1</v>
       </c>
       <c r="K37" s="4">
@@ -32461,7 +31763,7 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="69"/>
-      <c r="B38" s="77"/>
+      <c r="B38" s="87"/>
       <c r="C38" s="65"/>
       <c r="D38" s="4" t="s">
         <v>1084</v>
@@ -32481,8 +31783,8 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I38" s="74"/>
-      <c r="J38" s="87"/>
+      <c r="I38" s="77"/>
+      <c r="J38" s="80"/>
       <c r="K38" s="4">
         <v>1</v>
       </c>
@@ -32492,7 +31794,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="69"/>
-      <c r="B39" s="77"/>
+      <c r="B39" s="87"/>
       <c r="C39" s="65"/>
       <c r="D39" s="4" t="s">
         <v>1085</v>
@@ -32512,8 +31814,8 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I39" s="74"/>
-      <c r="J39" s="87"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="80"/>
       <c r="K39" s="4">
         <v>1</v>
       </c>
@@ -32523,7 +31825,7 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="69"/>
-      <c r="B40" s="77"/>
+      <c r="B40" s="87"/>
       <c r="C40" s="65"/>
       <c r="D40" s="4" t="s">
         <v>1086</v>
@@ -32543,8 +31845,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I40" s="74"/>
-      <c r="J40" s="87"/>
+      <c r="I40" s="77"/>
+      <c r="J40" s="80"/>
       <c r="K40" s="4">
         <v>1</v>
       </c>
@@ -32554,7 +31856,7 @@
     </row>
     <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="69"/>
-      <c r="B41" s="78"/>
+      <c r="B41" s="88"/>
       <c r="C41" s="71"/>
       <c r="D41" s="7" t="s">
         <v>1087</v>
@@ -32574,8 +31876,8 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="I41" s="75"/>
-      <c r="J41" s="88"/>
+      <c r="I41" s="78"/>
+      <c r="J41" s="81"/>
       <c r="K41" s="4">
         <v>1</v>
       </c>
@@ -32585,6 +31887,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="J27:J31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="J32:J36"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="J22:J26"/>
     <mergeCell ref="A2:A41"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
@@ -32601,373 +31920,8 @@
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="C17:C21"/>
     <mergeCell ref="I17:I21"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="J22:J26"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="I37:I41"/>
-    <mergeCell ref="J37:J41"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="C27:C31"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="J27:J31"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="J32:J36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="18" id="{B37CD624-61ED-45E3-B6FA-EA9F0F3CF88A}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="17" id="{B2E374CE-C122-45A4-A3E8-BA5B0A584D36}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K12:K16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="16" id="{F4C6C778-8060-4087-8FDA-8437C2E3885D}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K17</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{345FD89E-9E5B-4E09-9315-1B51D3DF4C42}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K18</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="13" id="{3F565026-4C66-4420-A116-601B2A7EB296}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="12" id="{C7C99F6A-8A2A-4622-AD3D-87B01B5DDA16}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K20</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="14" id="{92324271-C6C7-493A-9F8B-E63557A8A7E8}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K21</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="11" id="{5FF371A6-21B9-461D-87AE-B0F5165D8709}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K22</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="10" id="{442CA69F-B14F-4DB3-9A48-CFDCBE99AB87}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K23</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{8A569BBB-1DCB-4567-BF86-DB448516B537}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="9" id="{3831F9C1-7233-42A5-A21D-F38D18B41C8E}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K25</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{4407232F-D6F0-4271-917E-3FF30B8645F6}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K26</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{9E09A1C3-C709-4B83-9A43-E584F97BA814}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{9AD22BDD-1203-4B14-B0EA-821B6E7E9EC8}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{17FB8CFB-B6BE-4AB0-A427-BD0C087A19E1}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K29</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{C62E4E00-3A14-46F9-A595-14586CDBA56B}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K30</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{94EE13BF-F4E1-4A74-B83D-BF3E33039CD5}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{50042A8F-5505-429D-9057-445CFAAA1136}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K32:K41</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -33021,7 +31975,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="95" t="s">
         <v>1088</v>
       </c>
       <c r="B2" s="89" t="s">
@@ -33061,7 +32015,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="94"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="90"/>
       <c r="C3" s="65"/>
       <c r="D3" s="4" t="s">
@@ -33091,7 +32045,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="94"/>
+      <c r="A4" s="96"/>
       <c r="B4" s="90"/>
       <c r="C4" s="65"/>
       <c r="D4" s="4" t="s">
@@ -33121,7 +32075,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="94"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="90"/>
       <c r="C5" s="65"/>
       <c r="D5" s="4" t="s">
@@ -33151,7 +32105,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="94"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="91"/>
       <c r="C6" s="66"/>
       <c r="D6" s="4" t="s">
@@ -33181,7 +32135,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="94"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="89" t="s">
         <v>1094</v>
       </c>
@@ -33219,7 +32173,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="94"/>
+      <c r="A8" s="96"/>
       <c r="B8" s="90"/>
       <c r="C8" s="65"/>
       <c r="D8" s="4" t="s">
@@ -33249,7 +32203,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="94"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="90"/>
       <c r="C9" s="65"/>
       <c r="D9" s="4" t="s">
@@ -33279,7 +32233,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="94"/>
+      <c r="A10" s="96"/>
       <c r="B10" s="90"/>
       <c r="C10" s="65"/>
       <c r="D10" s="4" t="s">
@@ -33309,7 +32263,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="94"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="91"/>
       <c r="C11" s="66"/>
       <c r="D11" s="4" t="s">
@@ -33339,7 +32293,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="94"/>
+      <c r="A12" s="96"/>
       <c r="B12" s="89" t="s">
         <v>1099</v>
       </c>
@@ -33377,7 +32331,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="94"/>
+      <c r="A13" s="96"/>
       <c r="B13" s="90"/>
       <c r="C13" s="65"/>
       <c r="D13" s="4" t="s">
@@ -33407,7 +32361,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="94"/>
+      <c r="A14" s="96"/>
       <c r="B14" s="90"/>
       <c r="C14" s="65"/>
       <c r="D14" s="4" t="s">
@@ -33437,7 +32391,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="94"/>
+      <c r="A15" s="96"/>
       <c r="B15" s="90"/>
       <c r="C15" s="65"/>
       <c r="D15" s="4" t="s">
@@ -33467,7 +32421,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="94"/>
+      <c r="A16" s="96"/>
       <c r="B16" s="90"/>
       <c r="C16" s="65"/>
       <c r="D16" s="4" t="s">
@@ -33497,7 +32451,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="94"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="91"/>
       <c r="C17" s="66"/>
       <c r="D17" s="4" t="s">
@@ -33527,7 +32481,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="94"/>
+      <c r="A18" s="96"/>
       <c r="B18" s="89" t="s">
         <v>1105</v>
       </c>
@@ -33565,7 +32519,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="94"/>
+      <c r="A19" s="96"/>
       <c r="B19" s="90"/>
       <c r="C19" s="65"/>
       <c r="D19" s="12">
@@ -33595,7 +32549,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="94"/>
+      <c r="A20" s="96"/>
       <c r="B20" s="90"/>
       <c r="C20" s="65"/>
       <c r="D20" s="4" t="s">
@@ -33625,7 +32579,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="94"/>
+      <c r="A21" s="96"/>
       <c r="B21" s="90"/>
       <c r="C21" s="65"/>
       <c r="D21" s="4" t="s">
@@ -33655,7 +32609,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="94"/>
+      <c r="A22" s="96"/>
       <c r="B22" s="91"/>
       <c r="C22" s="66"/>
       <c r="D22" s="4" t="s">
@@ -33685,7 +32639,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="94"/>
+      <c r="A23" s="96"/>
       <c r="B23" s="89" t="s">
         <v>1108</v>
       </c>
@@ -33723,7 +32677,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="94"/>
+      <c r="A24" s="96"/>
       <c r="B24" s="90"/>
       <c r="C24" s="65"/>
       <c r="D24" s="4" t="s">
@@ -33753,7 +32707,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="94"/>
+      <c r="A25" s="96"/>
       <c r="B25" s="90"/>
       <c r="C25" s="65"/>
       <c r="D25" s="4" t="s">
@@ -33783,7 +32737,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="94"/>
+      <c r="A26" s="96"/>
       <c r="B26" s="90"/>
       <c r="C26" s="65"/>
       <c r="D26" s="4" t="s">
@@ -33813,7 +32767,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="94"/>
+      <c r="A27" s="96"/>
       <c r="B27" s="91"/>
       <c r="C27" s="66"/>
       <c r="D27" s="4" t="s">
@@ -33843,7 +32797,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="94"/>
+      <c r="A28" s="96"/>
       <c r="B28" s="89" t="s">
         <v>1113</v>
       </c>
@@ -33881,7 +32835,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="94"/>
+      <c r="A29" s="96"/>
       <c r="B29" s="90"/>
       <c r="C29" s="65"/>
       <c r="D29" s="4" t="s">
@@ -33911,7 +32865,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="94"/>
+      <c r="A30" s="96"/>
       <c r="B30" s="90"/>
       <c r="C30" s="65"/>
       <c r="D30" s="4" t="s">
@@ -33941,7 +32895,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="94"/>
+      <c r="A31" s="96"/>
       <c r="B31" s="90"/>
       <c r="C31" s="65"/>
       <c r="D31" s="4" t="s">
@@ -33971,7 +32925,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="94"/>
+      <c r="A32" s="96"/>
       <c r="B32" s="91"/>
       <c r="C32" s="66"/>
       <c r="D32" s="4" t="s">
@@ -34001,7 +32955,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="94"/>
+      <c r="A33" s="96"/>
       <c r="B33" s="89" t="s">
         <v>1118</v>
       </c>
@@ -34039,7 +32993,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="94"/>
+      <c r="A34" s="96"/>
       <c r="B34" s="90"/>
       <c r="C34" s="65"/>
       <c r="D34" s="4" t="s">
@@ -34069,7 +33023,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="94"/>
+      <c r="A35" s="96"/>
       <c r="B35" s="90"/>
       <c r="C35" s="65"/>
       <c r="D35" s="4" t="s">
@@ -34099,7 +33053,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="95"/>
+      <c r="A36" s="97"/>
       <c r="B36" s="91"/>
       <c r="C36" s="66"/>
       <c r="D36" s="4" t="s">
@@ -34130,6 +33084,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="C18:C22"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="J18:J22"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="I33:I36"/>
+    <mergeCell ref="J33:J36"/>
+    <mergeCell ref="I23:I27"/>
+    <mergeCell ref="J23:J27"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="I28:I32"/>
+    <mergeCell ref="J28:J32"/>
     <mergeCell ref="A2:A36"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
@@ -34146,46 +33113,8 @@
     <mergeCell ref="I12:I17"/>
     <mergeCell ref="J12:J17"/>
     <mergeCell ref="B18:B22"/>
-    <mergeCell ref="C18:C22"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="J18:J22"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="I33:I36"/>
-    <mergeCell ref="J33:J36"/>
-    <mergeCell ref="I23:I27"/>
-    <mergeCell ref="J23:J27"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="I28:I32"/>
-    <mergeCell ref="J28:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{DDD980D9-12C4-4BFD-B18E-698A900DB2F6}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -35606,31 +34535,6 @@
     <mergeCell ref="C27:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{3F4E788B-0F03-4C32-968B-BEF60D4FDE2A}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -37048,31 +35952,6 @@
     <mergeCell ref="C24:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{38719915-DE1C-48F4-8976-0BE8B31A06B6}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -38480,31 +37359,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{94C8DA97-F92E-4EB4-9D25-C900A9E44520}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -40306,31 +39160,6 @@
     <mergeCell ref="C37:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="38" id="{AE898859-2C9B-4804-8178-351686E1B3B8}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K46</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -41749,31 +40578,6 @@
     <mergeCell ref="C22:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{1FBD1160-5E75-4F4E-8037-B679AE94C494}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K36</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -43028,31 +41832,6 @@
     <mergeCell ref="C22:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{85F9A2E9-74C9-4592-BBF6-1A47D68658FF}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K31</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -44854,30 +43633,5 @@
     <mergeCell ref="C22:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{9B0747E0-3648-42A8-869F-F74E53976B45}">
-            <x14:iconSet iconSet="3Symbols2" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K2:K46</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>